<commit_message>
Improving the readability of class code ExcelTable, InternetTariff, WebParser
</commit_message>
<xml_diff>
--- a/samples/tariffs.xlsx
+++ b/samples/tariffs.xlsx
@@ -1458,7 +1458,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="C63" t="n">
         <v>50</v>
@@ -1474,7 +1474,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="C64" t="n">
         <v>100</v>
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="C65" t="n">
         <v>150</v>
@@ -1554,7 +1554,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="C69" t="n">
         <v>50</v>
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="C70" t="n">
         <v>100</v>
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>237</v>
+        <v>298</v>
       </c>
       <c r="C71" t="n">
         <v>150</v>
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>298</v>
+        <v>233</v>
       </c>
       <c r="C72" t="n">
         <v>50</v>
@@ -1618,7 +1618,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>298</v>
+        <v>233</v>
       </c>
       <c r="C73" t="n">
         <v>100</v>
@@ -1634,7 +1634,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>298</v>
+        <v>233</v>
       </c>
       <c r="C74" t="n">
         <v>150</v>
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>298</v>
+        <v>219</v>
       </c>
       <c r="C75" t="n">
         <v>50</v>
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>298</v>
+        <v>219</v>
       </c>
       <c r="C76" t="n">
         <v>100</v>
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>298</v>
+        <v>219</v>
       </c>
       <c r="C77" t="n">
         <v>150</v>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C78" t="n">
         <v>50</v>
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C79" t="n">
         <v>100</v>
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C80" t="n">
         <v>150</v>
@@ -1746,7 +1746,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C81" t="n">
         <v>50</v>
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C82" t="n">
         <v>100</v>
@@ -1778,7 +1778,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C83" t="n">
         <v>150</v>
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="C84" t="n">
         <v>50</v>
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="C85" t="n">
         <v>100</v>
@@ -1826,7 +1826,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="C86" t="n">
         <v>150</v>
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C87" t="n">
         <v>50</v>
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C88" t="n">
         <v>100</v>
@@ -1874,7 +1874,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="C89" t="n">
         <v>150</v>
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="C90" t="n">
         <v>50</v>
@@ -1906,7 +1906,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="C91" t="n">
         <v>100</v>
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="C92" t="n">
         <v>150</v>
@@ -1938,7 +1938,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="C93" t="n">
         <v>50</v>
@@ -1954,7 +1954,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="C94" t="n">
         <v>100</v>
@@ -1970,7 +1970,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>271</v>
+        <v>302</v>
       </c>
       <c r="C95" t="n">
         <v>150</v>

</xml_diff>